<commit_message>
changes and status report
</commit_message>
<xml_diff>
--- a/Documentation/EZ_Parts_Budget.xlsx
+++ b/Documentation/EZ_Parts_Budget.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="80">
   <si>
     <t>Description</t>
   </si>
@@ -240,6 +240,30 @@
   </si>
   <si>
     <t>ADA1982</t>
+  </si>
+  <si>
+    <t>15cm 90 degree micro USB cable</t>
+  </si>
+  <si>
+    <t>Micro USB Cable</t>
+  </si>
+  <si>
+    <t>CERRXIAN</t>
+  </si>
+  <si>
+    <t>B073PQWY2B</t>
+  </si>
+  <si>
+    <t>Power Source</t>
+  </si>
+  <si>
+    <t>APC 5000mAh battery pack</t>
+  </si>
+  <si>
+    <t>M5BK</t>
+  </si>
+  <si>
+    <t>APC</t>
   </si>
 </sst>
 </file>
@@ -640,11 +664,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G20"/>
+  <dimension ref="A1:G22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F8" sqref="F8"/>
+      <selection pane="bottomLeft" activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1052,17 +1076,63 @@
         <v>14.99</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="7" t="s">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="C19" s="3">
+        <v>2</v>
+      </c>
+      <c r="D19" s="14">
+        <v>10.99</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="F19" s="13" t="s">
+        <v>75</v>
+      </c>
+      <c r="G19" s="14">
+        <v>10.99</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="C20" s="3">
+        <v>1</v>
+      </c>
+      <c r="D20" s="14">
+        <v>34</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="F20" s="13" t="s">
+        <v>78</v>
+      </c>
+      <c r="G20" s="14">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="G19" s="6">
-        <f>SUM(G3:G18)</f>
-        <v>277.89</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="9"/>
+      <c r="G21" s="6">
+        <f>SUM(G3:G20)</f>
+        <v>322.88</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="9"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -1081,9 +1151,11 @@
     <hyperlink ref="F18" r:id="rId13"/>
     <hyperlink ref="F7" r:id="rId14"/>
     <hyperlink ref="F8" r:id="rId15"/>
+    <hyperlink ref="F19" r:id="rId16"/>
+    <hyperlink ref="F20" r:id="rId17"/>
   </hyperlinks>
   <printOptions gridLines="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="landscape" r:id="rId16"/>
+  <pageSetup orientation="landscape" r:id="rId18"/>
 </worksheet>
 </file>
</xml_diff>